<commit_message>
own account fund transfe test case added
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginData.xlsx
+++ b/src/test/resources/LoginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BS00865\IdeaProjects\Abbl\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BS00865\excel2\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9277CA-B6EC-4284-B828-34B7128013E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615D2ED6-7433-4BD2-9CB1-82B89F644AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -28,29 +28,28 @@
     <t>Password</t>
   </si>
   <si>
-    <t>shamsaldin</t>
+    <t>123456@Aa</t>
   </si>
   <si>
-    <t>123456@Ff</t>
-  </si>
-  <si>
-    <t>wronguser</t>
-  </si>
-  <si>
-    <t>shamsaldina</t>
-  </si>
-  <si>
-    <t>1234756@Ff</t>
+    <t>Shams1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,14 +87,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -396,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -408,43 +410,26 @@
     <col min="2" max="2" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{5B39D97B-B1AD-4DB9-94F5-672DADADB37C}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>